<commit_message>
Tuesday: Added some Cool Stuff
</commit_message>
<xml_diff>
--- a/Wireframe-2ndPlan.xlsx
+++ b/Wireframe-2ndPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darren Smith\bootcamp\Jan-25-bootcampwork\week-2\W2-S3-FlexBox\challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darren Smith\bootcamp\Jan-25-bootcampwork\week-2\W2-S3-FlexBox\challenge\DarrenMultiPagePortfolioWeek2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E0935E-E27D-4FD5-8B4D-7BD966C6E140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F6AFB5-C2DF-4DB2-918A-E8AC06178F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="0" windowWidth="17280" windowHeight="12336" activeTab="1" xr2:uid="{9BC9E7C6-5E36-4D69-8E51-B94122987F83}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9BC9E7C6-5E36-4D69-8E51-B94122987F83}"/>
   </bookViews>
   <sheets>
     <sheet name="Home New idea" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
   <si>
     <t>Logo</t>
   </si>
@@ -51,13 +51,7 @@
     <t>Footer: Darren Smith Copyright 2025</t>
   </si>
   <si>
-    <t>Projects / Recent</t>
-  </si>
-  <si>
     <t>About Me</t>
-  </si>
-  <si>
-    <t>Photo</t>
   </si>
   <si>
     <t>Text</t>
@@ -70,6 +64,18 @@
   </si>
   <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>Some text</t>
+  </si>
+  <si>
+    <t>Image Gallery of Projects</t>
+  </si>
+  <si>
+    <t>Contact Form</t>
+  </si>
+  <si>
+    <t>Banner</t>
   </si>
 </sst>
 </file>
@@ -193,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -210,11 +216,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -223,14 +224,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,16 +543,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1F739A-D2A5-4A4A-9387-E97C590C1DEA}">
-  <dimension ref="B2:P26"/>
+  <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -569,34 +567,29 @@
       <c r="M3" s="2"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12" t="s">
+      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="12"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -611,55 +604,29 @@
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="12"/>
-      <c r="P6" s="12"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="16"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="25"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -671,13 +638,11 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="26"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M10" s="23"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -689,55 +654,22 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="25"/>
+      <c r="M11" s="2"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="24"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="24"/>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="24"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -749,36 +681,23 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="26"/>
+      <c r="M15" s="7"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="24"/>
-    </row>
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="25"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="2"/>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
@@ -786,43 +705,40 @@
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="12"/>
       <c r="G18" s="1"/>
       <c r="H18" s="2"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="12"/>
       <c r="K18" s="1"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="28"/>
+      <c r="M18" s="3"/>
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="12"/>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="12"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="12"/>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
       <c r="I19" s="5"/>
-      <c r="J19" s="12"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="12"/>
+      <c r="L19" t="s">
+        <v>3</v>
+      </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="12"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="12"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="12"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="12"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="12"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
     </row>
@@ -831,11 +747,9 @@
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="12"/>
       <c r="G21" s="6"/>
       <c r="H21" s="7"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="12"/>
       <c r="K21" s="6"/>
       <c r="L21" s="7"/>
       <c r="M21" s="8"/>
@@ -874,19 +788,18 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="12"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
       <c r="N25" s="5"/>
     </row>
     <row r="26" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -911,16 +824,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0821E072-AF76-478A-B834-3B5F81CC0DB0}">
-  <dimension ref="B2:P26"/>
+  <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -934,39 +847,30 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12" t="s">
+      <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="12"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-    </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -980,10 +884,8 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -997,313 +899,274 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="18"/>
-      <c r="C7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="14" t="s">
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="15"/>
+      <c r="C7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="15"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="15"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="18"/>
-      <c r="C8" s="14" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-    </row>
-    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="18"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-    </row>
-    <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="18"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="20"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
-      <c r="M15" s="8"/>
+      <c r="M15" s="22"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="12"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="15"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="22"/>
       <c r="N16" s="5"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="12"/>
+    </row>
+    <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="15"/>
+      <c r="C17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="22"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="15"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
       <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="12"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="12"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="15"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="12"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="15"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
       <c r="N20" s="5"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B21" s="18"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="12"/>
+    </row>
+    <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="15"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="12"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="15"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
       <c r="N22" s="5"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-    </row>
-    <row r="23" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="18"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
+    </row>
+    <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="15"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
       <c r="M23" s="7"/>
       <c r="N23" s="8"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1317,29 +1180,24 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="12"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-    </row>
-    <row r="26" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1353,8 +1211,6 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1364,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45851BE-AD2A-4DE5-A44A-D8272D345D89}">
-  <dimension ref="B1:L18"/>
+  <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J16:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1393,18 +1249,23 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
-      <c r="E4" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="22" t="s">
         <v>3</v>
       </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
       <c r="L4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1422,47 +1283,270 @@
       <c r="K5" s="7"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="22"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="22"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="22"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="22"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="22"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="22"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="22"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="22"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="22"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="22"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="22"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="22"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="22"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="22"/>
+    </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="22"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="22"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="22"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="22"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="22"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="22"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="22"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="22"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="22"/>
+    </row>
+    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="22"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="22"/>
+    </row>
+    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="4"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="10"/>
-    </row>
-    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1471,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391A21C3-9405-4C48-94FA-52A7401C0744}">
-  <dimension ref="B1:L18"/>
+  <dimension ref="B1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1529,47 +1613,282 @@
       <c r="K5" s="7"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="4"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="4"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="10"/>
-    </row>
-    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>